<commit_message>
added negative algorithm added 3 new charts for negative algorithm added new chapters for report output file for negative algorithm
</commit_message>
<xml_diff>
--- a/sbh_analiza.xlsx
+++ b/sbh_analiza.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="24720" windowHeight="12075" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="24720" windowHeight="12075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="positive" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <definedName name="output_gn." localSheetId="0">positive!$K$2:$K$26</definedName>
     <definedName name="output_gnnt._1" localSheetId="2">truncation_negative!$A$2:$D$30</definedName>
     <definedName name="output_gp." localSheetId="0">positive!$A$1:$E$25</definedName>
+    <definedName name="output_n." localSheetId="1">negative!$A$34:$H$62</definedName>
     <definedName name="output_p." localSheetId="0">positive!$G$2:$K$25</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -85,7 +86,30 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="output_p" type="6" refreshedVersion="3" background="1" saveData="1">
+  <connection id="4" name="output_n" type="6" refreshedVersion="3" background="1" saveData="1">
+    <textPr codePage="852" sourceFile="C:\Users\Mateusz\Desktop\sbh\output_n." delimited="0" decimal="," thousands=" ">
+      <textFields count="17">
+        <textField type="skip"/>
+        <textField position="12"/>
+        <textField type="skip" position="17"/>
+        <textField position="21"/>
+        <textField type="skip" position="26"/>
+        <textField position="30"/>
+        <textField type="skip" position="35"/>
+        <textField position="39"/>
+        <textField type="skip" position="44"/>
+        <textField position="48"/>
+        <textField type="skip" position="56"/>
+        <textField position="57"/>
+        <textField type="skip" position="65"/>
+        <textField position="66"/>
+        <textField type="skip" position="74"/>
+        <textField position="75"/>
+        <textField type="skip" position="84"/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" name="output_p" type="6" refreshedVersion="3" background="1" saveData="1">
     <textPr codePage="852" sourceFile="C:\Users\Mateusz\Desktop\sbh\output_p." delimited="0" decimal="," thousands=" ">
       <textFields count="18">
         <textField/>
@@ -113,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="65">
   <si>
     <t>N</t>
   </si>
@@ -270,6 +294,45 @@
   <si>
     <t>GENERAL_NO_TRUNC</t>
   </si>
+  <si>
+    <t>NEGATIVE</t>
+  </si>
+  <si>
+    <t>120 [200]</t>
+  </si>
+  <si>
+    <t>160 [200]</t>
+  </si>
+  <si>
+    <t>180 [300]</t>
+  </si>
+  <si>
+    <t>240 [300]</t>
+  </si>
+  <si>
+    <t>300 [500]</t>
+  </si>
+  <si>
+    <t>320 [400]</t>
+  </si>
+  <si>
+    <t>400 [500]</t>
+  </si>
+  <si>
+    <t>468 [500]</t>
+  </si>
+  <si>
+    <t>488 [500]</t>
+  </si>
+  <si>
+    <t>492 [500]</t>
+  </si>
+  <si>
+    <t>498 [500]</t>
+  </si>
+  <si>
+    <t>482 [500]</t>
+  </si>
 </sst>
 </file>
 
@@ -425,13 +488,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="74352128"/>
-        <c:axId val="75218944"/>
+        <c:axId val="58390784"/>
+        <c:axId val="59449728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74352128"/>
+        <c:axId val="58390784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -456,8 +518,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.88503584578429462"/>
-              <c:y val="0.68423592884222806"/>
+              <c:x val="0.88503584578429451"/>
+              <c:y val="0.68423592884222795"/>
             </c:manualLayout>
           </c:layout>
         </c:title>
@@ -467,14 +529,14 @@
         <c:spPr>
           <a:ln w="28575"/>
         </c:spPr>
-        <c:crossAx val="75218944"/>
+        <c:crossAx val="59449728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75218944"/>
+        <c:axId val="59449728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="17.5"/>
@@ -508,7 +570,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="74352128"/>
+        <c:crossAx val="58390784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -517,7 +579,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -634,11 +696,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="78998144"/>
-        <c:axId val="79147776"/>
+        <c:axId val="59502592"/>
+        <c:axId val="59504512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="78998144"/>
+        <c:axId val="59502592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -668,14 +730,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79147776"/>
+        <c:crossAx val="59504512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79147776"/>
+        <c:axId val="59504512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -685,7 +747,7 @@
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78998144"/>
+        <c:crossAx val="59502592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -694,7 +756,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -724,13 +786,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL"/>
-              <a:t>dla</a:t>
+              <a:t>dla instancji z błędami negatywnymi</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="pl-PL" baseline="0"/>
-              <a:t> instancji z błędami negatywnymi</a:t>
-            </a:r>
-            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -745,49 +802,48 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:cat>
-            <c:numRef>
-              <c:f>negative!$J$7:$U$7</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
+            <c:strRef>
+              <c:f>negative!$J$38:$U$38</c:f>
+              <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>120</c:v>
+                  <c:v>120 [200]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>160</c:v>
+                  <c:v>160 [200]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>180</c:v>
+                  <c:v>180 [300]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>240</c:v>
+                  <c:v>240 [300]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>300</c:v>
+                  <c:v>300 [500]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>320</c:v>
+                  <c:v>320 [400]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>400</c:v>
+                  <c:v>400 [500]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>468</c:v>
+                  <c:v>468 [500]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>482</c:v>
+                  <c:v>482 [500]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>488</c:v>
+                  <c:v>488 [500]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>492</c:v>
+                  <c:v>492 [500]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>498</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>498 [500]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -835,12 +891,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="82520704"/>
-        <c:axId val="82556416"/>
+        <c:axId val="74540544"/>
+        <c:axId val="74589312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82520704"/>
+        <c:axId val="74540544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -856,12 +911,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>liczba słów w</a:t>
+                  <a:t>liczba słów w spektrum [liczba</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="pl-PL" baseline="0"/>
-                  <a:t> spektrum</a:t>
+                  <a:t> słów sekwencji]</a:t>
                 </a:r>
+                <a:endParaRPr lang="pl-PL"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -870,14 +926,14 @@
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82556416"/>
+        <c:crossAx val="74589312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82556416"/>
+        <c:axId val="74589312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -887,7 +943,7 @@
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82520704"/>
+        <c:crossAx val="74540544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -896,7 +952,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -951,49 +1007,48 @@
             <c:trendlineType val="linear"/>
           </c:trendline>
           <c:cat>
-            <c:numRef>
-              <c:f>negative!$J$7:$U$7</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
+            <c:strRef>
+              <c:f>negative!$J$38:$U$38</c:f>
+              <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>120</c:v>
+                  <c:v>120 [200]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>160</c:v>
+                  <c:v>160 [200]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>180</c:v>
+                  <c:v>180 [300]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>240</c:v>
+                  <c:v>240 [300]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>300</c:v>
+                  <c:v>300 [500]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>320</c:v>
+                  <c:v>320 [400]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>400</c:v>
+                  <c:v>400 [500]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>468</c:v>
+                  <c:v>468 [500]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>482</c:v>
+                  <c:v>482 [500]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>488</c:v>
+                  <c:v>488 [500]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>492</c:v>
+                  <c:v>492 [500]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>498</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>498 [500]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1041,11 +1096,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="71045504"/>
-        <c:axId val="71047040"/>
+        <c:axId val="61517824"/>
+        <c:axId val="61519744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="71045504"/>
+        <c:axId val="61517824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1061,7 +1116,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>liczba słów w spektrum</a:t>
+                  <a:t>liczba słów w spektrum [liczba słów sekwencji]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1070,14 +1125,14 @@
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71047040"/>
+        <c:crossAx val="61519744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71047040"/>
+        <c:axId val="61519744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1108,7 +1163,7 @@
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71045504"/>
+        <c:crossAx val="61517824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1117,13 +1172,741 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Procentowe wykorzystanie słów</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>dla</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> instancji z błędami negatywnymi</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Algorytm 4</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>negative!$J$38:$U$38</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>120 [200]</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>160 [200]</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>180 [300]</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>240 [300]</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300 [500]</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>320 [400]</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400 [500]</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>468 [500]</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>482 [500]</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>488 [500]</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>492 [500]</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>498 [500]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>negative!$J$41:$U$41</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.99722222222222223</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98958333333333337</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99555555555555564</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99479166666666663</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99170124481327804</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.97336065573770492</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.96951219512195119</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.96987951807228912</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="74862592"/>
+        <c:axId val="74864896"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="74862592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>liczba słów w</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> spektrum [liczba słów sekwencji]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="74864896"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="74864896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="74862592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Procentowe wykorzystanie słów</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>dla</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> instancji z błędami negatywnymi</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Algorytm 3</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>negative!$J$38:$U$38</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>120 [200]</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>160 [200]</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>180 [300]</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>240 [300]</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300 [500]</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>320 [400]</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400 [500]</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>468 [500]</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>482 [500]</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>488 [500]</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>492 [500]</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>498 [500]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>negative!$J$9:$U$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.9277777777777777</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.90416666666666656</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95370370370370361</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.94236111111111109</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.94333333333333336</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.94895833333333335</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.94416666666666671</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99572649572649574</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99170124481327804</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.97336065573770492</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.96951219512195119</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.96987951807228912</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Algorytm 4</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>negative!$J$38:$U$38</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>120 [200]</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>160 [200]</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>180 [300]</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>240 [300]</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300 [500]</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>320 [400]</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400 [500]</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>468 [500]</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>482 [500]</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>488 [500]</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>492 [500]</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>498 [500]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>negative!$J$41:$U$41</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.99722222222222223</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98958333333333337</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99555555555555564</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99479166666666663</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99170124481327804</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.97336065573770492</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.96951219512195119</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.96987951807228912</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="93799168"/>
+        <c:axId val="94081024"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="93799168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>liczba słów w</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> spektrum [liczba słów sekwencji]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="94081024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="94081024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="93799168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:style val="5"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Niewykorzystane słowa</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>dla instancji z błędami negatywnymi</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Niewykorzystane słowa</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>negative!$J$38:$U$38</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>120 [200]</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>160 [200]</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>180 [300]</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>240 [300]</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300 [500]</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>320 [400]</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400 [500]</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>468 [500]</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>482 [500]</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>488 [500]</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>492 [500]</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>498 [500]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>negative!$J$43:$U$43</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="59992704"/>
+        <c:axId val="85790080"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="59992704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>liczba słów w spektrum [liczba</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> słów sekwencji]</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="85790080"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="85790080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>liczba</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> niewykorzystanych słów</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="59992704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pl-PL"/>
   <c:chart>
@@ -1307,11 +2090,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="79148160"/>
-        <c:axId val="79894784"/>
+        <c:axId val="62706048"/>
+        <c:axId val="62707968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="79148160"/>
+        <c:axId val="62706048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1351,14 +2134,14 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79894784"/>
+        <c:crossAx val="62707968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79894784"/>
+        <c:axId val="62707968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1366,7 +2149,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79148160"/>
+        <c:crossAx val="62706048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1379,7 +2162,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1512,6 +2295,96 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1628775</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Wykres 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1704975</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Wykres 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Wykres 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1551,18 +2424,22 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="output_p." connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="output_gp." connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="output_p." connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="output_gn." connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="output_gp." connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="output_n." connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="output_gnnt._1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -2878,20 +3755,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U31"/>
+  <dimension ref="A1:V63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G30"/>
+    <sheetView tabSelected="1" topLeftCell="G49" workbookViewId="0">
+      <selection activeCell="R39" sqref="R39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.875" customWidth="1"/>
+    <col min="3" max="3" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2917,7 +3801,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:22">
       <c r="A2">
         <v>120</v>
       </c>
@@ -2943,7 +3827,7 @@
         <v>7.6369999999999993E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:22">
       <c r="A3">
         <v>120</v>
       </c>
@@ -2969,7 +3853,7 @@
         <v>7.7831999999999998E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:22">
       <c r="A4">
         <v>120</v>
       </c>
@@ -2995,7 +3879,7 @@
         <v>9.1363E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:22">
       <c r="A5">
         <v>160</v>
       </c>
@@ -3021,7 +3905,7 @@
         <v>7.4840000000000004E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:22">
       <c r="A6">
         <v>160</v>
       </c>
@@ -3047,7 +3931,7 @@
         <v>5.9674999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:22">
       <c r="A7">
         <v>160</v>
       </c>
@@ -3109,7 +3993,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:22">
       <c r="A8">
         <v>180</v>
       </c>
@@ -3183,7 +4067,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:22">
       <c r="A9">
         <v>180</v>
       </c>
@@ -3259,8 +4143,9 @@
         <f t="shared" si="0"/>
         <v>0.96987951807228912</v>
       </c>
-    </row>
-    <row r="10" spans="1:21">
+      <c r="V9" s="2"/>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10">
         <v>180</v>
       </c>
@@ -3337,7 +4222,7 @@
         <v>9.2071E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:22">
       <c r="A11">
         <v>240</v>
       </c>
@@ -3414,7 +4299,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:22">
       <c r="A12">
         <v>240</v>
       </c>
@@ -3440,7 +4325,7 @@
         <v>0.16273000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:22">
       <c r="A13">
         <v>240</v>
       </c>
@@ -3466,7 +4351,7 @@
         <v>0.41748400000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:22">
       <c r="A14">
         <v>240</v>
       </c>
@@ -3492,7 +4377,7 @@
         <v>0.22831000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:22">
       <c r="A15">
         <v>240</v>
       </c>
@@ -3518,7 +4403,7 @@
         <v>0.54066099999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:22">
       <c r="A16">
         <v>240</v>
       </c>
@@ -3913,9 +4798,1042 @@
         <v>13</v>
       </c>
     </row>
+    <row r="34" spans="1:22">
+      <c r="A34">
+        <v>120</v>
+      </c>
+      <c r="B34">
+        <v>200</v>
+      </c>
+      <c r="C34">
+        <v>209</v>
+      </c>
+      <c r="D34">
+        <v>120</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>6.8812999999999999E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22">
+      <c r="A35">
+        <v>120</v>
+      </c>
+      <c r="B35">
+        <v>200</v>
+      </c>
+      <c r="C35">
+        <v>209</v>
+      </c>
+      <c r="D35">
+        <v>119</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>8.2586999999999994E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22">
+      <c r="A36">
+        <v>120</v>
+      </c>
+      <c r="B36">
+        <v>200</v>
+      </c>
+      <c r="C36">
+        <v>207</v>
+      </c>
+      <c r="D36">
+        <v>120</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>8.4766999999999995E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22">
+      <c r="A37">
+        <v>160</v>
+      </c>
+      <c r="B37">
+        <v>200</v>
+      </c>
+      <c r="C37">
+        <v>209</v>
+      </c>
+      <c r="D37">
+        <v>155</v>
+      </c>
+      <c r="E37">
+        <v>5</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>5</v>
+      </c>
+      <c r="H37">
+        <v>7.4387999999999996E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22">
+      <c r="A38">
+        <v>160</v>
+      </c>
+      <c r="B38">
+        <v>200</v>
+      </c>
+      <c r="C38">
+        <v>209</v>
+      </c>
+      <c r="D38">
+        <v>160</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>5.3286E-2</v>
+      </c>
+      <c r="J38" t="s">
+        <v>53</v>
+      </c>
+      <c r="K38" t="s">
+        <v>54</v>
+      </c>
+      <c r="L38" t="s">
+        <v>55</v>
+      </c>
+      <c r="M38" t="s">
+        <v>56</v>
+      </c>
+      <c r="N38" t="s">
+        <v>57</v>
+      </c>
+      <c r="O38" t="s">
+        <v>58</v>
+      </c>
+      <c r="P38" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>60</v>
+      </c>
+      <c r="R38" t="s">
+        <v>64</v>
+      </c>
+      <c r="S38" t="s">
+        <v>61</v>
+      </c>
+      <c r="T38" t="s">
+        <v>62</v>
+      </c>
+      <c r="U38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22">
+      <c r="A39">
+        <v>160</v>
+      </c>
+      <c r="B39">
+        <v>200</v>
+      </c>
+      <c r="C39">
+        <v>207</v>
+      </c>
+      <c r="D39">
+        <v>160</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>6.9405999999999995E-2</v>
+      </c>
+      <c r="J39" s="1">
+        <v>120</v>
+      </c>
+      <c r="K39" s="1">
+        <v>160</v>
+      </c>
+      <c r="L39" s="1">
+        <v>180</v>
+      </c>
+      <c r="M39" s="1">
+        <v>240</v>
+      </c>
+      <c r="N39" s="1">
+        <v>300</v>
+      </c>
+      <c r="O39" s="1">
+        <v>320</v>
+      </c>
+      <c r="P39" s="1">
+        <v>400</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>468</v>
+      </c>
+      <c r="R39" s="1">
+        <v>482</v>
+      </c>
+      <c r="S39" s="1">
+        <v>488</v>
+      </c>
+      <c r="T39" s="1">
+        <v>492</v>
+      </c>
+      <c r="U39" s="1">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22">
+      <c r="A40">
+        <v>180</v>
+      </c>
+      <c r="B40">
+        <v>300</v>
+      </c>
+      <c r="C40">
+        <v>309</v>
+      </c>
+      <c r="D40">
+        <v>180</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0.20588300000000001</v>
+      </c>
+      <c r="I40" t="s">
+        <v>8</v>
+      </c>
+      <c r="J40" s="1">
+        <f>AVERAGE(D34:D36)</f>
+        <v>119.66666666666667</v>
+      </c>
+      <c r="K40" s="1">
+        <f>AVERAGE(D37:D39)</f>
+        <v>158.33333333333334</v>
+      </c>
+      <c r="L40" s="1">
+        <f>AVERAGE(D40:D42)</f>
+        <v>180</v>
+      </c>
+      <c r="M40" s="1">
+        <f>AVERAGE(D43:D48)</f>
+        <v>240</v>
+      </c>
+      <c r="N40" s="1">
+        <f>AVERAGE(D49:D51)</f>
+        <v>298.66666666666669</v>
+      </c>
+      <c r="O40" s="1">
+        <f>AVERAGE(D52:D54)</f>
+        <v>318.33333333333331</v>
+      </c>
+      <c r="P40" s="1">
+        <f>AVERAGE(D55:D57)</f>
+        <v>398</v>
+      </c>
+      <c r="Q40" s="1">
+        <f>AVERAGE(D58)</f>
+        <v>468</v>
+      </c>
+      <c r="R40" s="1">
+        <f>D59</f>
+        <v>478</v>
+      </c>
+      <c r="S40" s="1">
+        <v>475</v>
+      </c>
+      <c r="T40" s="1">
+        <v>477</v>
+      </c>
+      <c r="U40" s="1">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22">
+      <c r="A41">
+        <v>180</v>
+      </c>
+      <c r="B41">
+        <v>300</v>
+      </c>
+      <c r="C41">
+        <v>308</v>
+      </c>
+      <c r="D41">
+        <v>180</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0.178505</v>
+      </c>
+      <c r="I41" t="s">
+        <v>9</v>
+      </c>
+      <c r="J41" s="2">
+        <f>J40/J39</f>
+        <v>0.99722222222222223</v>
+      </c>
+      <c r="K41" s="2">
+        <f t="shared" ref="K41:U41" si="1">K40/K39</f>
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="L41" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M41" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N41" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99555555555555564</v>
+      </c>
+      <c r="O41" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99479166666666663</v>
+      </c>
+      <c r="P41" s="2">
+        <f t="shared" si="1"/>
+        <v>0.995</v>
+      </c>
+      <c r="Q41" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R41" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99170124481327804</v>
+      </c>
+      <c r="S41" s="2">
+        <f t="shared" si="1"/>
+        <v>0.97336065573770492</v>
+      </c>
+      <c r="T41" s="2">
+        <f t="shared" si="1"/>
+        <v>0.96951219512195119</v>
+      </c>
+      <c r="U41" s="2">
+        <f t="shared" si="1"/>
+        <v>0.96987951807228912</v>
+      </c>
+      <c r="V41" s="2"/>
+    </row>
+    <row r="42" spans="1:22">
+      <c r="A42">
+        <v>180</v>
+      </c>
+      <c r="B42">
+        <v>300</v>
+      </c>
+      <c r="C42">
+        <v>309</v>
+      </c>
+      <c r="D42">
+        <v>180</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0.188474</v>
+      </c>
+      <c r="I42" t="s">
+        <v>16</v>
+      </c>
+      <c r="J42">
+        <f>AVERAGE(H34:H36)</f>
+        <v>7.8722333333333325E-2</v>
+      </c>
+      <c r="K42">
+        <f>AVERAGE(H37:H39)</f>
+        <v>6.569333333333334E-2</v>
+      </c>
+      <c r="L42">
+        <f>AVERAGE(H40:H42)</f>
+        <v>0.19095399999999998</v>
+      </c>
+      <c r="M42">
+        <f>AVERAGE(H43:H48)</f>
+        <v>0.29838366666666666</v>
+      </c>
+      <c r="N42">
+        <f>AVERAGE(H49:H51)</f>
+        <v>0.78500533333333333</v>
+      </c>
+      <c r="O42">
+        <f>AVERAGE(H52:H54)</f>
+        <v>0.41373233333333337</v>
+      </c>
+      <c r="P42">
+        <f>AVERAGE(H55:H57)</f>
+        <v>0.68332833333333332</v>
+      </c>
+      <c r="Q42">
+        <f>H58</f>
+        <v>9.5244999999999996E-2</v>
+      </c>
+      <c r="R42">
+        <f>H59</f>
+        <v>9.3595999999999999E-2</v>
+      </c>
+      <c r="S42">
+        <f>H60</f>
+        <v>9.2989000000000002E-2</v>
+      </c>
+      <c r="T42">
+        <f>H61</f>
+        <v>9.7114000000000006E-2</v>
+      </c>
+      <c r="U42">
+        <f>H62</f>
+        <v>9.3852000000000005E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22">
+      <c r="A43">
+        <v>240</v>
+      </c>
+      <c r="B43">
+        <v>300</v>
+      </c>
+      <c r="C43">
+        <v>309</v>
+      </c>
+      <c r="D43">
+        <v>240</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0.184561</v>
+      </c>
+      <c r="I43" t="s">
+        <v>17</v>
+      </c>
+      <c r="J43" s="1">
+        <f>AVERAGE(G34:G36)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K43" s="1">
+        <f>AVERAGE(G37:G39)</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="L43" s="1">
+        <f>AVERAGE(G40:G42)</f>
+        <v>0</v>
+      </c>
+      <c r="M43" s="1">
+        <f>AVERAGE(G43:G48)</f>
+        <v>0</v>
+      </c>
+      <c r="N43" s="1">
+        <f>AVERAGE(G49:G51)</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="O43" s="1">
+        <f>AVERAGE(G52:G54)</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="P43" s="1">
+        <f>AVERAGE(G55:G57)</f>
+        <v>2</v>
+      </c>
+      <c r="Q43" s="1">
+        <f>G58</f>
+        <v>0</v>
+      </c>
+      <c r="R43" s="1">
+        <f>G59</f>
+        <v>4</v>
+      </c>
+      <c r="S43" s="1">
+        <f>G60</f>
+        <v>2</v>
+      </c>
+      <c r="T43" s="1">
+        <f>G61</f>
+        <v>13</v>
+      </c>
+      <c r="U43" s="1">
+        <f>G62</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22">
+      <c r="A44">
+        <v>240</v>
+      </c>
+      <c r="B44">
+        <v>300</v>
+      </c>
+      <c r="C44">
+        <v>309</v>
+      </c>
+      <c r="D44">
+        <v>240</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0.14913999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22">
+      <c r="A45">
+        <v>240</v>
+      </c>
+      <c r="B45">
+        <v>400</v>
+      </c>
+      <c r="C45">
+        <v>408</v>
+      </c>
+      <c r="D45">
+        <v>240</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0.34862900000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22">
+      <c r="A46">
+        <v>240</v>
+      </c>
+      <c r="B46">
+        <v>300</v>
+      </c>
+      <c r="C46">
+        <v>309</v>
+      </c>
+      <c r="D46">
+        <v>240</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0.213365</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22">
+      <c r="A47">
+        <v>240</v>
+      </c>
+      <c r="B47">
+        <v>400</v>
+      </c>
+      <c r="C47">
+        <v>408</v>
+      </c>
+      <c r="D47">
+        <v>240</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0.49476199999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22">
+      <c r="A48">
+        <v>240</v>
+      </c>
+      <c r="B48">
+        <v>400</v>
+      </c>
+      <c r="C48">
+        <v>409</v>
+      </c>
+      <c r="D48">
+        <v>240</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0.39984500000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49">
+        <v>300</v>
+      </c>
+      <c r="B49">
+        <v>500</v>
+      </c>
+      <c r="C49">
+        <v>509</v>
+      </c>
+      <c r="D49">
+        <v>299</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49">
+        <v>0.83841500000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50">
+        <v>300</v>
+      </c>
+      <c r="B50">
+        <v>500</v>
+      </c>
+      <c r="C50">
+        <v>507</v>
+      </c>
+      <c r="D50">
+        <v>300</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0.685442</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51">
+        <v>300</v>
+      </c>
+      <c r="B51">
+        <v>500</v>
+      </c>
+      <c r="C51">
+        <v>509</v>
+      </c>
+      <c r="D51">
+        <v>297</v>
+      </c>
+      <c r="E51">
+        <v>3</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>3</v>
+      </c>
+      <c r="H51">
+        <v>0.83115899999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52">
+        <v>320</v>
+      </c>
+      <c r="B52">
+        <v>400</v>
+      </c>
+      <c r="C52">
+        <v>409</v>
+      </c>
+      <c r="D52">
+        <v>315</v>
+      </c>
+      <c r="E52">
+        <v>5</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>5</v>
+      </c>
+      <c r="H52">
+        <v>0.41324</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53">
+        <v>320</v>
+      </c>
+      <c r="B53">
+        <v>400</v>
+      </c>
+      <c r="C53">
+        <v>408</v>
+      </c>
+      <c r="D53">
+        <v>320</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>0.43330200000000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54">
+        <v>320</v>
+      </c>
+      <c r="B54">
+        <v>400</v>
+      </c>
+      <c r="C54">
+        <v>409</v>
+      </c>
+      <c r="D54">
+        <v>320</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0.39465499999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55">
+        <v>400</v>
+      </c>
+      <c r="B55">
+        <v>500</v>
+      </c>
+      <c r="C55">
+        <v>509</v>
+      </c>
+      <c r="D55">
+        <v>394</v>
+      </c>
+      <c r="E55">
+        <v>6</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>6</v>
+      </c>
+      <c r="H55">
+        <v>0.66418900000000003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56">
+        <v>400</v>
+      </c>
+      <c r="B56">
+        <v>500</v>
+      </c>
+      <c r="C56">
+        <v>509</v>
+      </c>
+      <c r="D56">
+        <v>400</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0.694519</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57">
+        <v>400</v>
+      </c>
+      <c r="B57">
+        <v>500</v>
+      </c>
+      <c r="C57">
+        <v>509</v>
+      </c>
+      <c r="D57">
+        <v>400</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0.69127700000000003</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58">
+        <v>468</v>
+      </c>
+      <c r="B58">
+        <v>500</v>
+      </c>
+      <c r="C58">
+        <v>506</v>
+      </c>
+      <c r="D58">
+        <v>468</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>13</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>9.5244999999999996E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59">
+        <v>482</v>
+      </c>
+      <c r="B59">
+        <v>500</v>
+      </c>
+      <c r="C59">
+        <v>509</v>
+      </c>
+      <c r="D59">
+        <v>478</v>
+      </c>
+      <c r="E59">
+        <v>4</v>
+      </c>
+      <c r="F59">
+        <v>16</v>
+      </c>
+      <c r="G59">
+        <v>4</v>
+      </c>
+      <c r="H59">
+        <v>9.3595999999999999E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60">
+        <v>488</v>
+      </c>
+      <c r="B60">
+        <v>500</v>
+      </c>
+      <c r="C60">
+        <v>509</v>
+      </c>
+      <c r="D60">
+        <v>486</v>
+      </c>
+      <c r="E60">
+        <v>2</v>
+      </c>
+      <c r="F60">
+        <v>2</v>
+      </c>
+      <c r="G60">
+        <v>2</v>
+      </c>
+      <c r="H60">
+        <v>9.2989000000000002E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61">
+        <v>492</v>
+      </c>
+      <c r="B61">
+        <v>500</v>
+      </c>
+      <c r="C61">
+        <v>509</v>
+      </c>
+      <c r="D61">
+        <v>479</v>
+      </c>
+      <c r="E61">
+        <v>13</v>
+      </c>
+      <c r="F61">
+        <v>2</v>
+      </c>
+      <c r="G61">
+        <v>13</v>
+      </c>
+      <c r="H61">
+        <v>9.7114000000000006E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62">
+        <v>498</v>
+      </c>
+      <c r="B62">
+        <v>500</v>
+      </c>
+      <c r="C62">
+        <v>509</v>
+      </c>
+      <c r="D62">
+        <v>487</v>
+      </c>
+      <c r="E62">
+        <v>11</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>11</v>
+      </c>
+      <c r="H62">
+        <v>9.3852000000000005E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="C63" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:H34">
-    <sortCondition ref="A2:A34"/>
+  <sortState ref="A34:H62">
+    <sortCondition ref="A34:A62"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3927,7 +5845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q32" sqref="Q32"/>
     </sheetView>
   </sheetViews>
@@ -3960,15 +5878,15 @@
         <v>23</v>
       </c>
       <c r="E2">
-        <f>B2+9</f>
+        <f t="shared" ref="E2:E30" si="0">B2+9</f>
         <v>209</v>
       </c>
       <c r="F2">
-        <f>C2-E2</f>
+        <f t="shared" ref="F2:F30" si="1">C2-E2</f>
         <v>7</v>
       </c>
       <c r="G2">
-        <f>A2/B2</f>
+        <f t="shared" ref="G2:G30" si="2">A2/B2</f>
         <v>0.6</v>
       </c>
       <c r="Q2">
@@ -3993,7 +5911,7 @@
         <v>7</v>
       </c>
       <c r="X2">
-        <f>Q2/R2</f>
+        <f t="shared" ref="X2:X30" si="3">Q2/R2</f>
         <v>0.6</v>
       </c>
     </row>
@@ -4011,15 +5929,15 @@
         <v>31</v>
       </c>
       <c r="E3">
-        <f>B3+9</f>
+        <f t="shared" si="0"/>
         <v>209</v>
       </c>
       <c r="F3">
-        <f>C3-E3</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="G3">
-        <f>A3/B3</f>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="Q3">
@@ -4044,7 +5962,7 @@
         <v>10</v>
       </c>
       <c r="X3">
-        <f>Q3/R3</f>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
     </row>
@@ -4062,15 +5980,15 @@
         <v>46</v>
       </c>
       <c r="E4">
-        <f>B4+9</f>
+        <f t="shared" si="0"/>
         <v>209</v>
       </c>
       <c r="F4">
-        <f>C4-E4</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="G4">
-        <f>A4/B4</f>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="Q4">
@@ -4095,7 +6013,7 @@
         <v>9</v>
       </c>
       <c r="X4">
-        <f>Q4/R4</f>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
     </row>
@@ -4113,15 +6031,15 @@
         <v>24</v>
       </c>
       <c r="E5">
-        <f>B5+9</f>
+        <f t="shared" si="0"/>
         <v>309</v>
       </c>
       <c r="F5">
-        <f>C5-E5</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="G5">
-        <f>A5/B5</f>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="Q5">
@@ -4146,7 +6064,7 @@
         <v>2</v>
       </c>
       <c r="X5">
-        <f>Q5/R5</f>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
     </row>
@@ -4164,15 +6082,15 @@
         <v>34</v>
       </c>
       <c r="E6">
-        <f>B6+9</f>
+        <f t="shared" si="0"/>
         <v>309</v>
       </c>
       <c r="F6">
-        <f>C6-E6</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="G6">
-        <f>A6/B6</f>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="I6" s="2">
@@ -4223,7 +6141,7 @@
         <v>11</v>
       </c>
       <c r="X6">
-        <f>Q6/R6</f>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
     </row>
@@ -4241,15 +6159,15 @@
         <v>38</v>
       </c>
       <c r="E7">
-        <f>B7+9</f>
+        <f t="shared" si="0"/>
         <v>309</v>
       </c>
       <c r="F7">
-        <f>C7-E7</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="G7">
-        <f>A7/B7</f>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="H7" t="s">
@@ -4305,7 +6223,7 @@
         <v>12</v>
       </c>
       <c r="X7">
-        <f>Q7/R7</f>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
     </row>
@@ -4323,15 +6241,15 @@
         <v>36</v>
       </c>
       <c r="E8">
-        <f>B8+9</f>
+        <f t="shared" si="0"/>
         <v>409</v>
       </c>
       <c r="F8">
-        <f>C8-E8</f>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="G8">
-        <f>A8/B8</f>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="H8" t="s">
@@ -4387,7 +6305,7 @@
         <v>19</v>
       </c>
       <c r="X8">
-        <f>Q8/R8</f>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
     </row>
@@ -4405,15 +6323,15 @@
         <v>41</v>
       </c>
       <c r="E9">
-        <f>B9+9</f>
+        <f t="shared" si="0"/>
         <v>409</v>
       </c>
       <c r="F9">
-        <f>C9-E9</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="G9">
-        <f>A9/B9</f>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="Q9">
@@ -4438,7 +6356,7 @@
         <v>7</v>
       </c>
       <c r="X9">
-        <f>Q9/R9</f>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
     </row>
@@ -4456,15 +6374,15 @@
         <v>43</v>
       </c>
       <c r="E10">
-        <f>B10+9</f>
+        <f t="shared" si="0"/>
         <v>409</v>
       </c>
       <c r="F10">
-        <f>C10-E10</f>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="G10">
-        <f>A10/B10</f>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="Q10">
@@ -4489,7 +6407,7 @@
         <v>17</v>
       </c>
       <c r="X10">
-        <f>Q10/R10</f>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
     </row>
@@ -4507,15 +6425,15 @@
         <v>19</v>
       </c>
       <c r="E11">
-        <f>B11+9</f>
+        <f t="shared" si="0"/>
         <v>509</v>
       </c>
       <c r="F11">
-        <f>C11-E11</f>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="G11">
-        <f>A11/B11</f>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="Q11">
@@ -4540,7 +6458,7 @@
         <v>17</v>
       </c>
       <c r="X11">
-        <f>Q11/R11</f>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
     </row>
@@ -4558,15 +6476,15 @@
         <v>27</v>
       </c>
       <c r="E12">
-        <f>B12+9</f>
+        <f t="shared" si="0"/>
         <v>509</v>
       </c>
       <c r="F12">
-        <f>C12-E12</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="G12">
-        <f>A12/B12</f>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="Q12">
@@ -4591,7 +6509,7 @@
         <v>21</v>
       </c>
       <c r="X12">
-        <f>Q12/R12</f>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
     </row>
@@ -4609,15 +6527,15 @@
         <v>33</v>
       </c>
       <c r="E13">
-        <f>B13+9</f>
+        <f t="shared" si="0"/>
         <v>509</v>
       </c>
       <c r="F13">
-        <f>C13-E13</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="G13">
-        <f>A13/B13</f>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="Q13">
@@ -4642,7 +6560,7 @@
         <v>13</v>
       </c>
       <c r="X13">
-        <f>Q13/R13</f>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
     </row>
@@ -4660,15 +6578,15 @@
         <v>22</v>
       </c>
       <c r="E14">
-        <f>B14+9</f>
+        <f t="shared" si="0"/>
         <v>209</v>
       </c>
       <c r="F14">
-        <f>C14-E14</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="G14">
-        <f>A14/B14</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="Q14">
@@ -4693,7 +6611,7 @@
         <v>13</v>
       </c>
       <c r="X14">
-        <f>Q14/R14</f>
+        <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
     </row>
@@ -4711,15 +6629,15 @@
         <v>30</v>
       </c>
       <c r="E15">
-        <f>B15+9</f>
+        <f t="shared" si="0"/>
         <v>209</v>
       </c>
       <c r="F15">
-        <f>C15-E15</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="G15">
-        <f>A15/B15</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="Q15">
@@ -4744,7 +6662,7 @@
         <v>15</v>
       </c>
       <c r="X15">
-        <f>Q15/R15</f>
+        <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
     </row>
@@ -4762,15 +6680,15 @@
         <v>45</v>
       </c>
       <c r="E16">
-        <f>B16+9</f>
+        <f t="shared" si="0"/>
         <v>209</v>
       </c>
       <c r="F16">
-        <f>C16-E16</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="G16">
-        <f>A16/B16</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="Q16">
@@ -4795,7 +6713,7 @@
         <v>18</v>
       </c>
       <c r="X16">
-        <f>Q16/R16</f>
+        <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
     </row>
@@ -4813,15 +6731,15 @@
         <v>25</v>
       </c>
       <c r="E17">
-        <f>B17+9</f>
+        <f t="shared" si="0"/>
         <v>309</v>
       </c>
       <c r="F17">
-        <f>C17-E17</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="G17">
-        <f>A17/B17</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="Q17">
@@ -4846,7 +6764,7 @@
         <v>14</v>
       </c>
       <c r="X17">
-        <f>Q17/R17</f>
+        <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
     </row>
@@ -4864,15 +6782,15 @@
         <v>35</v>
       </c>
       <c r="E18">
-        <f>B18+9</f>
+        <f t="shared" si="0"/>
         <v>309</v>
       </c>
       <c r="F18">
-        <f>C18-E18</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="G18">
-        <f>A18/B18</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="Q18">
@@ -4897,7 +6815,7 @@
         <v>13</v>
       </c>
       <c r="X18">
-        <f>Q18/R18</f>
+        <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
     </row>
@@ -4915,15 +6833,15 @@
         <v>39</v>
       </c>
       <c r="E19">
-        <f>B19+9</f>
+        <f t="shared" si="0"/>
         <v>309</v>
       </c>
       <c r="F19">
-        <f>C19-E19</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="G19">
-        <f>A19/B19</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="Q19">
@@ -4948,7 +6866,7 @@
         <v>13</v>
       </c>
       <c r="X19">
-        <f>Q19/R19</f>
+        <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
     </row>
@@ -4966,15 +6884,15 @@
         <v>37</v>
       </c>
       <c r="E20">
-        <f>B20+9</f>
+        <f t="shared" si="0"/>
         <v>409</v>
       </c>
       <c r="F20">
-        <f>C20-E20</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="G20">
-        <f>A20/B20</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="Q20">
@@ -4999,7 +6917,7 @@
         <v>15</v>
       </c>
       <c r="X20">
-        <f>Q20/R20</f>
+        <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
     </row>
@@ -5017,15 +6935,15 @@
         <v>42</v>
       </c>
       <c r="E21">
-        <f>B21+9</f>
+        <f t="shared" si="0"/>
         <v>409</v>
       </c>
       <c r="F21">
-        <f>C21-E21</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="G21">
-        <f>A21/B21</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="Q21">
@@ -5050,7 +6968,7 @@
         <v>23</v>
       </c>
       <c r="X21">
-        <f>Q21/R21</f>
+        <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
     </row>
@@ -5068,15 +6986,15 @@
         <v>44</v>
       </c>
       <c r="E22">
-        <f>B22+9</f>
+        <f t="shared" si="0"/>
         <v>409</v>
       </c>
       <c r="F22">
-        <f>C22-E22</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="G22">
-        <f>A22/B22</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="Q22">
@@ -5101,7 +7019,7 @@
         <v>11</v>
       </c>
       <c r="X22">
-        <f>Q22/R22</f>
+        <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
     </row>
@@ -5119,15 +7037,15 @@
         <v>18</v>
       </c>
       <c r="E23">
-        <f>B23+9</f>
+        <f t="shared" si="0"/>
         <v>509</v>
       </c>
       <c r="F23">
-        <f>C23-E23</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="G23">
-        <f>A23/B23</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="Q23">
@@ -5152,7 +7070,7 @@
         <v>20</v>
       </c>
       <c r="X23">
-        <f>Q23/R23</f>
+        <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
     </row>
@@ -5170,15 +7088,15 @@
         <v>26</v>
       </c>
       <c r="E24">
-        <f>B24+9</f>
+        <f t="shared" si="0"/>
         <v>509</v>
       </c>
       <c r="F24">
-        <f>C24-E24</f>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="G24">
-        <f>A24/B24</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="Q24">
@@ -5203,7 +7121,7 @@
         <v>23</v>
       </c>
       <c r="X24">
-        <f>Q24/R24</f>
+        <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
     </row>
@@ -5221,15 +7139,15 @@
         <v>32</v>
       </c>
       <c r="E25">
-        <f>B25+9</f>
+        <f t="shared" si="0"/>
         <v>509</v>
       </c>
       <c r="F25">
-        <f>C25-E25</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="G25">
-        <f>A25/B25</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="Q25">
@@ -5254,7 +7172,7 @@
         <v>24</v>
       </c>
       <c r="X25">
-        <f>Q25/R25</f>
+        <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
     </row>
@@ -5272,15 +7190,15 @@
         <v>29</v>
       </c>
       <c r="E26">
-        <f>B26+9</f>
+        <f t="shared" si="0"/>
         <v>509</v>
       </c>
       <c r="F26">
-        <f>C26-E26</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="G26">
-        <f>A26/B26</f>
+        <f t="shared" si="2"/>
         <v>0.93600000000000005</v>
       </c>
       <c r="Q26">
@@ -5305,7 +7223,7 @@
         <v>2</v>
       </c>
       <c r="X26">
-        <f>Q26/R26</f>
+        <f t="shared" si="3"/>
         <v>0.93600000000000005</v>
       </c>
     </row>
@@ -5323,15 +7241,15 @@
         <v>28</v>
       </c>
       <c r="E27">
-        <f>B27+9</f>
+        <f t="shared" si="0"/>
         <v>509</v>
       </c>
       <c r="F27">
-        <f>C27-E27</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="G27">
-        <f>A27/B27</f>
+        <f t="shared" si="2"/>
         <v>0.96399999999999997</v>
       </c>
       <c r="Q27">
@@ -5356,7 +7274,7 @@
         <v>4</v>
       </c>
       <c r="X27">
-        <f>Q27/R27</f>
+        <f t="shared" si="3"/>
         <v>0.96399999999999997</v>
       </c>
     </row>
@@ -5374,15 +7292,15 @@
         <v>21</v>
       </c>
       <c r="E28">
-        <f>B28+9</f>
+        <f t="shared" si="0"/>
         <v>509</v>
       </c>
       <c r="F28">
-        <f>C28-E28</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="G28">
-        <f>A28/B28</f>
+        <f t="shared" si="2"/>
         <v>0.97599999999999998</v>
       </c>
       <c r="Q28">
@@ -5407,7 +7325,7 @@
         <v>13</v>
       </c>
       <c r="X28">
-        <f>Q28/R28</f>
+        <f t="shared" si="3"/>
         <v>0.97599999999999998</v>
       </c>
     </row>
@@ -5425,15 +7343,15 @@
         <v>20</v>
       </c>
       <c r="E29">
-        <f>B29+9</f>
+        <f t="shared" si="0"/>
         <v>509</v>
       </c>
       <c r="F29">
-        <f>C29-E29</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="G29">
-        <f>A29/B29</f>
+        <f t="shared" si="2"/>
         <v>0.98399999999999999</v>
       </c>
       <c r="Q29">
@@ -5458,7 +7376,7 @@
         <v>15</v>
       </c>
       <c r="X29">
-        <f>Q29/R29</f>
+        <f t="shared" si="3"/>
         <v>0.98399999999999999</v>
       </c>
     </row>
@@ -5476,15 +7394,15 @@
         <v>40</v>
       </c>
       <c r="E30">
-        <f>B30+9</f>
+        <f t="shared" si="0"/>
         <v>509</v>
       </c>
       <c r="F30">
-        <f>C30-E30</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="G30">
-        <f>A30/B30</f>
+        <f t="shared" si="2"/>
         <v>0.996</v>
       </c>
       <c r="Q30">
@@ -5509,7 +7427,7 @@
         <v>15</v>
       </c>
       <c r="X30">
-        <f>Q30/R30</f>
+        <f t="shared" si="3"/>
         <v>0.996</v>
       </c>
     </row>

</xml_diff>